<commit_message>
Database changed, raw scores check is added
</commit_message>
<xml_diff>
--- a/Chemistry1.xlsx
+++ b/Chemistry1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>1=March, 2=June, 3=Septembe, 4=December</t>
   </si>
@@ -47,6 +47,9 @@
     <t>GENDER</t>
   </si>
   <si>
+    <t>ATTENDANCE</t>
+  </si>
+  <si>
     <t>SCORE</t>
   </si>
   <si>
@@ -57,6 +60,9 @@
   </si>
   <si>
     <t>AMIRI</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
   <si>
     <t>SELEMANI</t>
@@ -422,7 +428,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,12 +436,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -443,13 +449,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -457,7 +463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -476,96 +482,109 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>80</v>
       </c>
       <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
-      <c r="F10"/>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>